<commit_message>
Updated Northwind spreadsheet to completion
</commit_message>
<xml_diff>
--- a/NorthwindTablesAndColumns.xlsx
+++ b/NorthwindTablesAndColumns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\YUU-LearnToCode\DataAnalytics\week_9\W9_Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5DB17F6-DF02-4881-9DA9-6AA48DC8DF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC1A1171-F654-4BA8-9B61-63B34F6C4A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="95">
   <si>
     <t>table_name</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Customers</t>
   </si>
   <si>
-    <t>CompanyName</t>
-  </si>
-  <si>
     <t>ContactName</t>
   </si>
   <si>
@@ -314,6 +311,15 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>CompanyCountry</t>
+  </si>
+  <si>
+    <t>Sum, Avg, etc.</t>
   </si>
 </sst>
 </file>
@@ -702,10 +708,10 @@
   <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,31 +749,31 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -787,12 +793,27 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>91</v>
       </c>
     </row>
@@ -813,12 +834,27 @@
         <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>91</v>
       </c>
     </row>
@@ -839,13 +875,28 @@
         <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -865,13 +916,28 @@
         <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -891,12 +957,27 @@
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -908,7 +989,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>9</v>
@@ -917,12 +998,27 @@
         <v>80</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -934,7 +1030,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>9</v>
@@ -943,13 +1039,28 @@
         <v>60</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -960,7 +1071,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>
@@ -969,13 +1080,28 @@
         <v>60</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -986,7 +1112,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
@@ -995,12 +1121,27 @@
         <v>120</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1012,7 +1153,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>
@@ -1021,12 +1162,27 @@
         <v>30</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1038,7 +1194,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>9</v>
@@ -1047,12 +1203,27 @@
         <v>30</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1064,7 +1235,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>9</v>
@@ -1073,12 +1244,27 @@
         <v>20</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1090,7 +1276,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>9</v>
@@ -1099,12 +1285,27 @@
         <v>30</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1116,7 +1317,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>9</v>
@@ -1125,12 +1326,27 @@
         <v>48</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1142,7 +1358,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>9</v>
@@ -1151,24 +1367,39 @@
         <v>48</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>7</v>
@@ -1177,24 +1408,39 @@
         <v>4</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>9</v>
@@ -1203,21 +1449,39 @@
         <v>40</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
@@ -1226,21 +1490,39 @@
         <v>20</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1">
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>9</v>
@@ -1249,21 +1531,39 @@
         <v>60</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1">
         <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>9</v>
@@ -1272,67 +1572,121 @@
         <v>50</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1">
         <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="E22" s="1">
         <v>8</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" s="1">
         <v>8</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1">
         <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>9</v>
@@ -1341,21 +1695,39 @@
         <v>120</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="1">
         <v>9</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>9</v>
@@ -1364,21 +1736,39 @@
         <v>30</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1">
         <v>10</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>9</v>
@@ -1387,21 +1777,39 @@
         <v>30</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>9</v>
@@ -1410,21 +1818,39 @@
         <v>20</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1">
         <v>12</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>9</v>
@@ -1433,21 +1859,39 @@
         <v>30</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1">
         <v>13</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>9</v>
@@ -1456,21 +1900,39 @@
         <v>48</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="1">
         <v>14</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>9</v>
@@ -1479,21 +1941,39 @@
         <v>8</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="1">
         <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>13</v>
@@ -1502,21 +1982,39 @@
         <v>16</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="1">
         <v>16</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>11</v>
@@ -1525,21 +2023,39 @@
         <v>16</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" s="1">
         <v>17</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>7</v>
@@ -1548,21 +2064,39 @@
         <v>4</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="1">
         <v>18</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>9</v>
@@ -1571,21 +2105,39 @@
         <v>510</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="2">
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>7</v>
@@ -1594,24 +2146,39 @@
         <v>4</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" s="2">
         <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>9</v>
@@ -1620,24 +2187,39 @@
         <v>40</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1">
         <v>1</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>7</v>
@@ -1646,24 +2228,39 @@
         <v>4</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B38" s="1">
         <v>2</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>7</v>
@@ -1672,93 +2269,162 @@
         <v>4</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" s="1">
         <v>3</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="E39" s="1">
         <v>8</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" s="1">
         <v>4</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="E40" s="1">
         <v>2</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41" s="1">
         <v>5</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="E41" s="1">
         <v>4</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" s="2">
         <v>1</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>7</v>
@@ -1767,18 +2433,33 @@
         <v>4</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43" s="2">
         <v>2</v>
@@ -1793,24 +2474,39 @@
         <v>10</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44" s="2">
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>7</v>
@@ -1819,93 +2515,162 @@
         <v>4</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" s="2">
         <v>4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E45" s="2">
         <v>8</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" s="2">
         <v>5</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E46" s="2">
         <v>8</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" s="2">
         <v>6</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E47" s="2">
         <v>8</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" s="2">
         <v>7</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>7</v>
@@ -1914,44 +2679,80 @@
         <v>4</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" s="2">
         <v>8</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E49" s="2">
         <v>8</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" s="2">
         <v>9</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>9</v>
@@ -1960,21 +2761,39 @@
         <v>80</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" s="2">
         <v>10</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>9</v>
@@ -1983,21 +2802,39 @@
         <v>120</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" s="2">
         <v>11</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>9</v>
@@ -2006,21 +2843,39 @@
         <v>30</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" s="2">
         <v>12</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>9</v>
@@ -2029,21 +2884,39 @@
         <v>30</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" s="2">
         <v>13</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>9</v>
@@ -2052,21 +2925,39 @@
         <v>20</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" s="2">
         <v>14</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>9</v>
@@ -2075,21 +2966,39 @@
         <v>30</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B56" s="1">
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>7</v>
@@ -2098,24 +3007,39 @@
         <v>4</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B57" s="1">
         <v>2</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>9</v>
@@ -2124,21 +3048,39 @@
         <v>80</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B58" s="1">
         <v>3</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>7</v>
@@ -2147,18 +3089,33 @@
         <v>4</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B59" s="1">
         <v>4</v>
@@ -2173,24 +3130,39 @@
         <v>4</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60" s="1">
         <v>5</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>9</v>
@@ -2199,136 +3171,244 @@
         <v>40</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B61" s="1">
         <v>6</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="E61" s="1">
         <v>8</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B62" s="1">
         <v>7</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E62" s="1">
         <v>2</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B63" s="1">
         <v>8</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E63" s="1">
         <v>2</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64" s="1">
         <v>9</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E64" s="1">
         <v>2</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65" s="1">
         <v>10</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="E65" s="1">
         <v>1</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B66" s="2">
         <v>1</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>7</v>
@@ -2337,24 +3417,39 @@
         <v>4</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M66" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B67" s="2">
         <v>2</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>15</v>
@@ -2363,21 +3458,39 @@
         <v>100</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M67" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B68" s="1">
         <v>1</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>7</v>
@@ -2386,24 +3499,39 @@
         <v>4</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B69" s="1">
         <v>2</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>9</v>
@@ -2412,21 +3540,39 @@
         <v>80</v>
       </c>
       <c r="F69" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G69" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J69" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B70" s="1">
         <v>3</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>9</v>
@@ -2435,21 +3581,39 @@
         <v>48</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M70" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B71" s="2">
         <v>1</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>7</v>
@@ -2458,24 +3622,39 @@
         <v>4</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M71" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" s="2">
         <v>2</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>9</v>
@@ -2484,21 +3663,39 @@
         <v>80</v>
       </c>
       <c r="F72" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I72" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G72" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J72" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B73" s="2">
         <v>3</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>9</v>
@@ -2507,21 +3704,39 @@
         <v>60</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M73" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B74" s="2">
         <v>4</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>9</v>
@@ -2530,21 +3745,39 @@
         <v>60</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M74" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B75" s="2">
         <v>5</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>9</v>
@@ -2553,21 +3786,39 @@
         <v>120</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M75" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B76" s="2">
         <v>6</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>9</v>
@@ -2576,21 +3827,39 @@
         <v>30</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M76" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77" s="2">
         <v>7</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>9</v>
@@ -2599,21 +3868,39 @@
         <v>30</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K77" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M77" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" s="2">
         <v>8</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>9</v>
@@ -2622,21 +3909,39 @@
         <v>20</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K78" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L78" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M78" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" s="2">
         <v>9</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>9</v>
@@ -2645,21 +3950,39 @@
         <v>30</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M79" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" s="2">
         <v>10</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>9</v>
@@ -2668,21 +3991,39 @@
         <v>48</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K80" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L80" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M80" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B81" s="2">
         <v>11</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>9</v>
@@ -2691,21 +4032,39 @@
         <v>48</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M81" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B82" s="2">
         <v>12</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>11</v>
@@ -2714,21 +4073,39 @@
         <v>16</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J82" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L82" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M82" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B83" s="1">
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>9</v>
@@ -2737,24 +4114,39 @@
         <v>40</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L83" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B84" s="1">
         <v>2</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>15</v>
@@ -2763,21 +4155,39 @@
         <v>100</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L84" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B85" s="1">
         <v>3</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>7</v>
@@ -2786,12 +4196,27 @@
         <v>4</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H85" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M85" s="1" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>